<commit_message>
[UPDATE] MATLAB file referred to the mu param
</commit_message>
<xml_diff>
--- a/caracterizacion/IdentFvsV.xlsx
+++ b/caracterizacion/IdentFvsV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\Semestre-10\Tecnicas de control\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d97dfd61da619a5/UNAL FORE/SEMESTRE 9/TECNICAS DE CONTROL/PROYECTO/eolic-balancing-cs/caracterizacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{319E57F2-0314-4F90-B9A4-B1B259DD5EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{319E57F2-0314-4F90-B9A4-B1B259DD5EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{832D2EAC-7C85-4192-926E-FAC68BE8648B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68AD6B39-C190-4FA2-BF87-25474CEEEEA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{68AD6B39-C190-4FA2-BF87-25474CEEEEA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -141,32 +141,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{C0E50B8B-0EC9-4B0B-B224-1F811510339F}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -181,7 +182,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -718,7 +719,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1246,7 +1247,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1765,7 +1766,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4651,7 +4652,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4949,20 +4950,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96FA629-7C01-4F0A-B2BD-324C250E098B}">
   <dimension ref="B2:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -4979,7 +4980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -4998,7 +4999,7 @@
         <v>7.2849060000000016E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>4.5665550000000008E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>1</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>1.5349330827067678E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -5132,7 +5133,7 @@
         <v>1.9037300751879718E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>3</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>3.3789180451127832E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>4</v>
       </c>
@@ -5212,7 +5213,7 @@
         <v>4.1165120300751895E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>5</v>
       </c>
@@ -5252,7 +5253,7 @@
         <v>5.5917000000000008E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>6</v>
       </c>
@@ -5292,7 +5293,7 @@
         <v>8.9108729323308281E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>7</v>
       </c>
@@ -5332,7 +5333,7 @@
         <v>0.12672602255639101</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>8</v>
       </c>
@@ -5372,7 +5373,7 @@
         <v>0.1643433157894737</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>9</v>
       </c>
@@ -5412,7 +5413,7 @@
         <v>0.19569106015037599</v>
       </c>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C21" s="6">
         <v>6</v>
       </c>
@@ -5424,7 +5425,7 @@
         <v>1.5349330827067678E-2</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C22" s="6">
         <v>8</v>
       </c>
@@ -5436,7 +5437,7 @@
         <v>1.9037300751879718E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C23" s="6">
         <v>12.5</v>
       </c>
@@ -5448,7 +5449,7 @@
         <v>3.3789180451127832E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C24" s="6">
         <v>15</v>
       </c>
@@ -5460,7 +5461,7 @@
         <v>4.1165120300751895E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C25" s="6">
         <v>20</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>5.5917000000000008E-2</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C26" s="6">
         <v>32</v>
       </c>
@@ -5484,7 +5485,7 @@
         <v>8.9108729323308281E-2</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C27" s="6">
         <v>55</v>
       </c>
@@ -5496,7 +5497,7 @@
         <v>0.12672602255639101</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C28" s="6">
         <v>75</v>
       </c>
@@ -5508,7 +5509,7 @@
         <v>0.1643433157894737</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C29" s="6">
         <v>90</v>
       </c>
@@ -5520,7 +5521,7 @@
         <v>0.19569106015037599</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>100</v>
       </c>
@@ -5532,7 +5533,7 @@
         <v>0.21893735267577075</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>0</v>
       </c>
@@ -5543,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C36" s="5">
         <v>3</v>
       </c>
@@ -5554,133 +5555,133 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" s="6">
-        <f>C21</f>
+        <f t="shared" ref="C37:E45" si="6">C21</f>
         <v>6</v>
       </c>
       <c r="D37" s="6">
-        <f>D21</f>
+        <f t="shared" si="6"/>
         <v>0.66</v>
       </c>
       <c r="E37" s="9">
-        <f>E21</f>
+        <f t="shared" si="6"/>
         <v>1.5349330827067678E-2</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="6">
-        <f>C22</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="D38" s="6">
-        <f>D22</f>
+        <f t="shared" si="6"/>
         <v>0.87</v>
       </c>
       <c r="E38" s="9">
-        <f>E22</f>
+        <f t="shared" si="6"/>
         <v>1.9037300751879718E-2</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" s="6">
-        <f>C23</f>
+        <f t="shared" si="6"/>
         <v>12.5</v>
       </c>
       <c r="D39" s="6">
-        <f>D23</f>
+        <f t="shared" si="6"/>
         <v>1.36</v>
       </c>
       <c r="E39" s="9">
-        <f>E23</f>
+        <f t="shared" si="6"/>
         <v>3.3789180451127832E-2</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C40" s="6">
-        <f>C24</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="D40" s="6">
-        <f>D24</f>
+        <f t="shared" si="6"/>
         <v>1.55</v>
       </c>
       <c r="E40" s="9">
-        <f>E24</f>
+        <f t="shared" si="6"/>
         <v>4.1165120300751895E-2</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C41" s="6">
-        <f>C25</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="D41" s="6">
-        <f>D25</f>
+        <f t="shared" si="6"/>
         <v>1.87</v>
       </c>
       <c r="E41" s="9">
-        <f>E25</f>
+        <f t="shared" si="6"/>
         <v>5.5917000000000008E-2</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C42" s="6">
-        <f>C26</f>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="D42" s="6">
-        <f>D26</f>
+        <f t="shared" si="6"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="E42" s="9">
-        <f>E26</f>
+        <f t="shared" si="6"/>
         <v>8.9108729323308281E-2</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C43" s="6">
-        <f>C27</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="D43" s="6">
-        <f>D27</f>
+        <f t="shared" si="6"/>
         <v>3.29</v>
       </c>
       <c r="E43" s="9">
-        <f>E27</f>
+        <f t="shared" si="6"/>
         <v>0.12672602255639101</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C44" s="6">
-        <f>C28</f>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="D44" s="6">
-        <f>D28</f>
+        <f t="shared" si="6"/>
         <v>3.95</v>
       </c>
       <c r="E44" s="9">
-        <f>E28</f>
+        <f t="shared" si="6"/>
         <v>0.1643433157894737</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C45" s="6">
-        <f>C29</f>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="D45" s="6">
-        <f>D29</f>
+        <f t="shared" si="6"/>
         <v>4.3899999999999997</v>
       </c>
       <c r="E45" s="9">
-        <f>E29</f>
+        <f t="shared" si="6"/>
         <v>0.19569106015037599</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>100</v>
       </c>
@@ -5692,26 +5693,26 @@
         <v>0.21893735267577075</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C47">
         <v>110</v>
       </c>
       <c r="D47">
         <v>5</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="2">
         <f>E46</f>
         <v>0.21893735267577075</v>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>120</v>
       </c>
       <c r="D48">
         <v>6</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="2">
         <f>E47</f>
         <v>0.21893735267577075</v>
       </c>

</xml_diff>